<commit_message>
bugfix e adição de diagramas
</commit_message>
<xml_diff>
--- a/planilha/Tabela de controle de versionamento.xlsx
+++ b/planilha/Tabela de controle de versionamento.xlsx
@@ -192,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -263,10 +263,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -364,9 +360,9 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.38"/>
@@ -484,8 +480,8 @@
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,7 +490,7 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,7 +499,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="17"/>
@@ -511,7 +507,7 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
-      <c r="F9" s="20"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="17"/>
@@ -519,7 +515,7 @@
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17"/>
@@ -527,7 +523,7 @@
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
-      <c r="F11" s="20"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="17"/>
@@ -535,7 +531,7 @@
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
-      <c r="F12" s="20"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17"/>
@@ -543,7 +539,7 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17"/>
@@ -551,23 +547,23 @@
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
-      <c r="F14" s="20"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="20"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="20"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>